<commit_message>
Note that w6 is remote
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B4EA70-4590-D346-932A-19E5C1AD2238}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC13DE3-6F62-0F4B-89BA-536061DE9144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -198,9 +198,6 @@
     <t>We will introduce parallel iterations (`purrr::map2()` and `purrr::pmap()`) and apply them within the context of list columns. We'll discuss the differences betweeen`purrr::map()` and `purrr::modify()` while introducing new functions, including `purrr::safely()`, and `purrr::walk()`. We will also discuss different types of loops, focusing mostly on `purrr::reduce()` (and noting the similarities with `base::Reduce()`).</t>
   </si>
   <si>
-    <t>Writing functions 1 &amp; 2</t>
-  </si>
-  <si>
     <t>The first part of this lecture will focus on the very basics of functions - understanding that everything in R is a function, the components of a function, when to write a function, and how to go about it (e.g., development and informal testing). We will then extend this discussion toward making the internals of a function more complicated, while still keeping functions as simple as possible. Functions within functions!</t>
   </si>
   <si>
@@ -274,6 +271,9 @@
   </si>
   <si>
     <t>w6</t>
+  </si>
+  <si>
+    <t>**REMOTE ONLY** Writing functions 1 &amp; 2</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <selection pane="topRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -761,7 +761,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>43</v>
@@ -793,7 +793,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>45</v>
@@ -831,7 +831,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>47</v>
@@ -870,7 +870,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
@@ -884,13 +884,13 @@
         <v>44683</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>31</v>
@@ -902,10 +902,10 @@
         <v>51</v>
       </c>
       <c r="K7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="M7" s="6"/>
     </row>
@@ -917,11 +917,11 @@
         <v>44690</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>34</v>
@@ -930,10 +930,10 @@
         <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>29</v>
@@ -948,10 +948,10 @@
         <v>44697</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
@@ -960,19 +960,19 @@
         <v>17</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -983,11 +983,11 @@
         <v>44704</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3"/>
       <c r="H10" s="3" t="s">
@@ -997,13 +997,13 @@
         <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H11" s="3"/>
       <c r="M11" s="1" t="s">

</xml_diff>

<commit_message>
post w1 lecture link
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC772DBC-3270-B944-B5B6-C5EE7BC88C88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB7C793-DA12-624E-A7DD-89CF99FC65BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>week</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>w7</t>
+  </si>
+  <si>
+    <t>https://youtu.be/owhV5SNC92Y</t>
   </si>
 </sst>
 </file>
@@ -660,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -752,6 +755,9 @@
       <c r="L2" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="M2" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1">

</xml_diff>

<commit_message>
post w8 and w9 slides
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB7C793-DA12-624E-A7DD-89CF99FC65BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD4752B-F0CA-3B44-883D-737DA6F202BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>week</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Shiny 1 &amp; 2</t>
   </si>
   <si>
-    <t>We will start by introducing the very basics of shiny - the user interface (UI) and the server. We will work together to create a basic shiny application, modifying the default template to use ggplot2. Shiny dashboards and different layout options will also be discussed.</t>
-  </si>
-  <si>
     <t>lab-3; assignments/#draft</t>
   </si>
   <si>
@@ -280,6 +277,15 @@
   </si>
   <si>
     <t>https://youtu.be/owhV5SNC92Y</t>
+  </si>
+  <si>
+    <t>Please clone [the course repo of example apps](https://github.com/datalorax/shiny-app-examples) before class.We will start by introducing the very basics of shiny - the user interface (UI) and the server. We will work together to create a basic shiny application, modifying the default template to use ggplot2. Shiny dashboards and different layout options will also be discussed.</t>
+  </si>
+  <si>
+    <t>w8</t>
+  </si>
+  <si>
+    <t>w9</t>
   </si>
 </sst>
 </file>
@@ -663,9 +669,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,7 +762,7 @@
         <v>41</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="85" x14ac:dyDescent="0.2">
@@ -770,7 +776,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>43</v>
@@ -802,7 +808,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>45</v>
@@ -840,7 +846,7 @@
         <v>54</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>47</v>
@@ -879,7 +885,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
@@ -893,10 +899,10 @@
         <v>44683</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>57</v>
@@ -929,7 +935,7 @@
         <v>60</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>61</v>
@@ -951,7 +957,7 @@
       </c>
       <c r="M8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="85" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -961,8 +967,11 @@
       <c r="C9" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>21</v>
@@ -971,19 +980,19 @@
         <v>17</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="153" x14ac:dyDescent="0.2">
@@ -994,11 +1003,13 @@
         <v>44704</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="F10" s="3"/>
       <c r="H10" s="3" t="s">
@@ -1008,13 +1019,13 @@
         <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -1029,7 +1040,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H11" s="3"/>
       <c r="M11" s="1" t="s">

</xml_diff>

<commit_message>
post w2 lecture recording
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD4752B-F0CA-3B44-883D-737DA6F202BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69EE8E2-0622-F742-ABBB-A99E66F14926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>week</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>w9</t>
+  </si>
+  <si>
+    <t>https://youtu.be/SCAm4oeJxL0</t>
   </si>
 </sst>
 </file>
@@ -669,9 +672,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,6 +799,9 @@
       <c r="L3" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="M3" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
post w3 lecture recording
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69EE8E2-0622-F742-ABBB-A99E66F14926}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68536257-D52B-9E4A-916D-17F3DF4878D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
   <si>
     <t>week</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>https://youtu.be/SCAm4oeJxL0</t>
+  </si>
+  <si>
+    <t>https://youtu.be/lUYc5ecxT5U</t>
   </si>
 </sst>
 </file>
@@ -674,7 +677,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M3" sqref="M3"/>
+      <selection pane="topRight" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,6 +843,9 @@
       <c r="L4" s="1">
         <v>25</v>
       </c>
+      <c r="M4" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="1">

</xml_diff>

<commit_message>
post w4 lecture video
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68536257-D52B-9E4A-916D-17F3DF4878D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045754A8-9944-CF4F-80C5-EAC0B6C50A20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="90">
   <si>
     <t>week</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>https://youtu.be/lUYc5ecxT5U</t>
+  </si>
+  <si>
+    <t>https://youtu.be/IVXJIgdnmrc</t>
   </si>
 </sst>
 </file>
@@ -675,9 +678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
       <pane xSplit="3" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M4" sqref="M4"/>
+      <selection pane="topRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,7 +887,9 @@
       <c r="L5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A6" s="1">

</xml_diff>

<commit_message>
post w6 lecture recording
</commit_message>
<xml_diff>
--- a/website-data/course-schedule.xlsx
+++ b/website-data/course-schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Teaching/data_sci_specialization/2021-22/c3-fp-2022/website-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E035C5B-118F-1044-9A99-CF0D54ED7147}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3F151B-C3B2-8C46-9CB1-CA3D329F89BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{9B46E7E8-B2FF-5244-8636-A2DC9407036E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="92">
   <si>
     <t>week</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>https://youtu.be/9Ebhv66PPZ4</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ViIKu6y3kWM</t>
   </si>
 </sst>
 </file>
@@ -681,9 +684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAD85F2-0528-6D42-B5EC-DC3A01653045}">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="167" zoomScaleNormal="68" workbookViewId="0">
+      <pane xSplit="3" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -945,7 +948,9 @@
       <c r="L7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="6"/>
+      <c r="M7" s="6" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="8" spans="1:13" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="1">

</xml_diff>